<commit_message>
- update test by switching `$(random|any|...)` to `$(random|alphanumeric|...)` to avoid HTML-conflicting randomized content
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_webmail.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_webmail.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="12645" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="28770" windowHeight="12435" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -1995,7 +1995,7 @@
   </si>
   <si>
     <t>Welcome! Glad you've joined us! 
-$(random|any|256)
+$(random|alphanumeric|256)
 &lt;a href="https://www.website.com/link?id=$(random|alphanumeric|64)"&gt;Get Started&lt;/a&gt;
 &lt;br/&gt;</t>
   </si>
@@ -2179,10 +2179,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -2254,7 +2254,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2262,23 +2262,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2293,7 +2277,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2307,75 +2291,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2391,7 +2322,76 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2424,13 +2424,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2442,19 +2448,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2466,37 +2460,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2514,13 +2502,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2538,73 +2592,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2731,17 +2731,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2757,21 +2763,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2811,6 +2802,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2828,7 +2828,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2846,128 +2846,128 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -5784,10 +5784,10 @@
   <sheetPr/>
   <dimension ref="A1:O203"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="15"/>
@@ -12837,10 +12837,10 @@
   <sheetPr/>
   <dimension ref="A1:O200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
- added additional waits for mails to arrive at mailinator.
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_webmail.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_webmail.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="703">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="708">
   <si>
     <t>target</t>
   </si>
@@ -2009,154 +2009,169 @@
     <t>let mailinator catch up</t>
   </si>
   <si>
-    <t>20000</t>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>mails</t>
+  </si>
+  <si>
+    <t>Welcome</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>${mails}</t>
   </si>
   <si>
     <t>Mailinator</t>
   </si>
   <si>
+    <t>we'll wait up to 5 minutes for all the mails to arrive</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>300000</t>
+  </si>
+  <si>
+    <t>[LIST(${mails}) =&gt; size]</t>
+  </si>
+  <si>
+    <t>wait and retry...</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
     <t>retrieve mail</t>
   </si>
   <si>
-    <t>mails</t>
-  </si>
-  <si>
-    <t>Welcome</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>${mails}</t>
+    <t>retrieve mail details</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>[LIST(${mails}) =&gt; item(${i})]</t>
+  </si>
+  <si>
+    <t>${mail}</t>
+  </si>
+  <si>
+    <t>assert expected value per mail</t>
+  </si>
+  <si>
+    <t>${mail}.id</t>
+  </si>
+  <si>
+    <t>${webmail.inbox}-</t>
+  </si>
+  <si>
+    <t>${mail}.subject</t>
+  </si>
+  <si>
+    <t>Welcome to the Club #</t>
+  </si>
+  <si>
+    <t>${MyMail.username}</t>
+  </si>
+  <si>
+    <t>${mail}.from</t>
+  </si>
+  <si>
+    <t>${mail}.to</t>
+  </si>
+  <si>
+    <t>${mail}.time</t>
+  </si>
+  <si>
+    <t>$(sysdate|now|yyyy-MM-dd)</t>
+  </si>
+  <si>
+    <t>${mail}.content</t>
+  </si>
+  <si>
+    <t>Welcome! Glad you've joined us!</t>
+  </si>
+  <si>
+    <t>[LIST(${mail}.links) =&gt; size]</t>
+  </si>
+  <si>
+    <t>detail mail</t>
+  </si>
+  <si>
+    <t>nexial.browser</t>
+  </si>
+  <si>
+    <t>chrome.headless</t>
+  </si>
+  <si>
+    <t>site.url</t>
+  </si>
+  <si>
+    <t>https://www.mailinator.com/</t>
+  </si>
+  <si>
+    <t>loc.nav-items</t>
+  </si>
+  <si>
+    <t>css=.wrapper-nav-items a</t>
+  </si>
+  <si>
+    <t>loc.email-link</t>
+  </si>
+  <si>
+    <t>css=.wrapper-nav-items a[aria-label='Email']</t>
+  </si>
+  <si>
+    <t>expected.email-link</t>
+  </si>
+  <si>
+    <t>https://www.mailinator.com/v4/public/inboxes.jsp</t>
+  </si>
+  <si>
+    <t>Go to Site</t>
+  </si>
+  <si>
+    <t>${site.url}</t>
+  </si>
+  <si>
+    <t>${loc.nav-items}</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
+    <t>${loc.email-link}</t>
+  </si>
+  <si>
+    <t>actual.email-link</t>
+  </si>
+  <si>
+    <t>href</t>
+  </si>
+  <si>
+    <t>Assert Email Link</t>
+  </si>
+  <si>
+    <t>${expected.email-link}</t>
+  </si>
+  <si>
+    <t>${actual.email-link}</t>
+  </si>
+  <si>
+    <t>${webmail2.inbox}@temporary-mail.net</t>
+  </si>
+  <si>
+    <t>Temporary-mail</t>
+  </si>
+  <si>
+    <t>webmail2</t>
   </si>
   <si>
     <t>assert all sent email are found</t>
-  </si>
-  <si>
-    <t>[LIST(${mails}) =&gt; size]</t>
-  </si>
-  <si>
-    <t>retrieve mail details</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>[LIST(${mails}) =&gt; item(${i})]</t>
-  </si>
-  <si>
-    <t>${mail}</t>
-  </si>
-  <si>
-    <t>assert expected value per mail</t>
-  </si>
-  <si>
-    <t>${mail}.id</t>
-  </si>
-  <si>
-    <t>${webmail.inbox}-</t>
-  </si>
-  <si>
-    <t>${mail}.subject</t>
-  </si>
-  <si>
-    <t>Welcome to the Club #</t>
-  </si>
-  <si>
-    <t>${MyMail.username}</t>
-  </si>
-  <si>
-    <t>${mail}.from</t>
-  </si>
-  <si>
-    <t>${mail}.to</t>
-  </si>
-  <si>
-    <t>${mail}.time</t>
-  </si>
-  <si>
-    <t>$(sysdate|now|yyyy-MM-dd)</t>
-  </si>
-  <si>
-    <t>${mail}.content</t>
-  </si>
-  <si>
-    <t>Welcome! Glad you've joined us!</t>
-  </si>
-  <si>
-    <t>[LIST(${mail}.links) =&gt; size]</t>
-  </si>
-  <si>
-    <t>detail mail</t>
-  </si>
-  <si>
-    <t>nexial.browser</t>
-  </si>
-  <si>
-    <t>chrome.headless</t>
-  </si>
-  <si>
-    <t>site.url</t>
-  </si>
-  <si>
-    <t>https://www.mailinator.com/</t>
-  </si>
-  <si>
-    <t>loc.nav-items</t>
-  </si>
-  <si>
-    <t>css=.wrapper-nav-items a</t>
-  </si>
-  <si>
-    <t>loc.email-link</t>
-  </si>
-  <si>
-    <t>css=.wrapper-nav-items a[aria-label='Email']</t>
-  </si>
-  <si>
-    <t>expected.email-link</t>
-  </si>
-  <si>
-    <t>https://www.mailinator.com/v4/public/inboxes.jsp</t>
-  </si>
-  <si>
-    <t>Go to Site</t>
-  </si>
-  <si>
-    <t>${site.url}</t>
-  </si>
-  <si>
-    <t>${loc.nav-items}</t>
-  </si>
-  <si>
-    <t>3000</t>
-  </si>
-  <si>
-    <t>${loc.email-link}</t>
-  </si>
-  <si>
-    <t>actual.email-link</t>
-  </si>
-  <si>
-    <t>href</t>
-  </si>
-  <si>
-    <t>Assert Email Link</t>
-  </si>
-  <si>
-    <t>${expected.email-link}</t>
-  </si>
-  <si>
-    <t>${actual.email-link}</t>
-  </si>
-  <si>
-    <t>${webmail2.inbox}@temporary-mail.net</t>
-  </si>
-  <si>
-    <t>Temporary-mail</t>
-  </si>
-  <si>
-    <t>webmail2</t>
   </si>
   <si>
     <t>delete just 5 emails</t>
@@ -2397,7 +2412,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2413,6 +2428,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.0499893185216834"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.05"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2828,7 +2849,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2847,28 +2868,28 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2886,22 +2907,22 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="35" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -2910,68 +2931,68 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3165,6 +3186,18 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -5782,12 +5815,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O203"/>
+  <dimension ref="A1:O207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="15"/>
@@ -6208,29 +6241,25 @@
       <c r="O15" s="21"/>
     </row>
     <row r="16" ht="23" customHeight="1" spans="1:15">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="18"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="53" t="s">
+        <v>123</v>
+      </c>
+      <c r="E16" s="53" t="s">
         <v>649</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>650</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>651</v>
       </c>
       <c r="F16" s="25" t="s">
         <v>29</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="I16" s="25"/>
       <c r="J16" s="32"/>
@@ -6242,15 +6271,15 @@
     </row>
     <row r="17" ht="23" customHeight="1" spans="1:15">
       <c r="A17" s="18"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="24" t="s">
+      <c r="B17" s="51"/>
+      <c r="C17" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="53" t="s">
         <v>426</v>
       </c>
-      <c r="E17" s="25" t="s">
-        <v>654</v>
+      <c r="E17" s="53" t="s">
+        <v>652</v>
       </c>
       <c r="F17" s="25"/>
       <c r="G17" s="25"/>
@@ -6263,22 +6292,24 @@
       <c r="N17" s="22"/>
       <c r="O17" s="21"/>
     </row>
-    <row r="18" ht="23" customHeight="1" spans="1:15">
-      <c r="A18" s="18"/>
-      <c r="B18" s="19" t="s">
+    <row r="18" ht="35" customHeight="1" spans="1:15">
+      <c r="A18" s="18" t="s">
+        <v>653</v>
+      </c>
+      <c r="B18" s="54" t="s">
+        <v>654</v>
+      </c>
+      <c r="C18" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="56" t="s">
+        <v>382</v>
+      </c>
+      <c r="E18" s="56" t="s">
         <v>655</v>
       </c>
-      <c r="C18" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="E18" s="25" t="s">
+      <c r="F18" s="25" t="s">
         <v>656</v>
-      </c>
-      <c r="F18" s="25" t="s">
-        <v>637</v>
       </c>
       <c r="G18" s="25"/>
       <c r="H18" s="25"/>
@@ -6292,18 +6323,18 @@
     </row>
     <row r="19" ht="23" customHeight="1" spans="1:15">
       <c r="A19" s="18"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>386</v>
+      <c r="B19" s="54"/>
+      <c r="C19" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="56" t="s">
+        <v>139</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>631</v>
-      </c>
-      <c r="F19" s="25" t="s">
-        <v>632</v>
+        <v>657</v>
+      </c>
+      <c r="F19" s="53" t="s">
+        <v>637</v>
       </c>
       <c r="G19" s="25"/>
       <c r="H19" s="25"/>
@@ -6317,21 +6348,19 @@
     </row>
     <row r="20" ht="23" customHeight="1" spans="1:15">
       <c r="A20" s="18"/>
-      <c r="B20" s="26" t="s">
-        <v>657</v>
-      </c>
-      <c r="C20" s="27" t="s">
+      <c r="B20" s="54" t="s">
+        <v>658</v>
+      </c>
+      <c r="C20" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="39" t="s">
-        <v>382</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>658</v>
-      </c>
-      <c r="F20" s="25" t="s">
-        <v>635</v>
-      </c>
+      <c r="D20" s="56" t="s">
+        <v>429</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>659</v>
+      </c>
+      <c r="F20" s="53"/>
       <c r="G20" s="25"/>
       <c r="H20" s="25"/>
       <c r="I20" s="25"/>
@@ -6342,23 +6371,28 @@
       <c r="N20" s="22"/>
       <c r="O20" s="21"/>
     </row>
-    <row r="21" ht="23" customHeight="1" spans="1:15">
-      <c r="A21" s="18"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="40" t="s">
-        <v>139</v>
-      </c>
-      <c r="E21" s="31" t="s">
-        <v>636</v>
+    <row r="21" ht="23" customHeight="1" spans="2:15">
+      <c r="B21" s="54" t="s">
+        <v>660</v>
+      </c>
+      <c r="C21" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="56" t="s">
+        <v>123</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>649</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>656</v>
-      </c>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
+        <v>29</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>650</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>651</v>
+      </c>
       <c r="I21" s="25"/>
       <c r="J21" s="32"/>
       <c r="K21" s="21"/>
@@ -6369,22 +6403,18 @@
     </row>
     <row r="22" ht="23" customHeight="1" spans="1:15">
       <c r="A22" s="18"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="40" t="s">
-        <v>93</v>
-      </c>
-      <c r="E22" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="G22" s="25" t="s">
-        <v>659</v>
-      </c>
+      <c r="B22" s="54"/>
+      <c r="C22" s="55" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="56" t="s">
+        <v>426</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>652</v>
+      </c>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
       <c r="H22" s="25"/>
       <c r="I22" s="25"/>
       <c r="J22" s="32"/>
@@ -6396,17 +6426,19 @@
     </row>
     <row r="23" ht="23" customHeight="1" spans="1:15">
       <c r="A23" s="18"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="30" t="s">
+      <c r="B23" s="19"/>
+      <c r="C23" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="40" t="s">
-        <v>426</v>
-      </c>
-      <c r="E23" s="31" t="s">
-        <v>660</v>
-      </c>
-      <c r="F23" s="25"/>
+      <c r="D23" s="25" t="s">
+        <v>386</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>631</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>632</v>
+      </c>
       <c r="G23" s="25"/>
       <c r="H23" s="25"/>
       <c r="I23" s="25"/>
@@ -6419,20 +6451,20 @@
     </row>
     <row r="24" ht="23" customHeight="1" spans="1:15">
       <c r="A24" s="18"/>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="26" t="s">
         <v>661</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="40" t="s">
-        <v>285</v>
-      </c>
-      <c r="E24" s="31" t="s">
+      <c r="D24" s="39" t="s">
+        <v>382</v>
+      </c>
+      <c r="E24" s="28" t="s">
         <v>662</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>663</v>
+        <v>635</v>
       </c>
       <c r="G24" s="25"/>
       <c r="H24" s="25"/>
@@ -6448,16 +6480,16 @@
       <c r="A25" s="18"/>
       <c r="B25" s="29"/>
       <c r="C25" s="30" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D25" s="40" t="s">
-        <v>285</v>
+        <v>139</v>
       </c>
       <c r="E25" s="31" t="s">
-        <v>664</v>
+        <v>636</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>665</v>
+        <v>657</v>
       </c>
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
@@ -6473,18 +6505,20 @@
       <c r="A26" s="18"/>
       <c r="B26" s="29"/>
       <c r="C26" s="30" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="E26" s="31" t="s">
-        <v>666</v>
+        <v>16</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>667</v>
-      </c>
-      <c r="G26" s="25"/>
+        <v>29</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>663</v>
+      </c>
       <c r="H26" s="25"/>
       <c r="I26" s="25"/>
       <c r="J26" s="32"/>
@@ -6501,14 +6535,12 @@
         <v>5</v>
       </c>
       <c r="D27" s="40" t="s">
-        <v>44</v>
+        <v>426</v>
       </c>
       <c r="E27" s="31" t="s">
-        <v>642</v>
-      </c>
-      <c r="F27" s="25" t="s">
-        <v>668</v>
-      </c>
+        <v>664</v>
+      </c>
+      <c r="F27" s="25"/>
       <c r="G27" s="25"/>
       <c r="H27" s="25"/>
       <c r="I27" s="25"/>
@@ -6521,7 +6553,9 @@
     </row>
     <row r="28" ht="23" customHeight="1" spans="1:15">
       <c r="A28" s="18"/>
-      <c r="B28" s="29"/>
+      <c r="B28" s="29" t="s">
+        <v>665</v>
+      </c>
       <c r="C28" s="30" t="s">
         <v>5</v>
       </c>
@@ -6529,10 +6563,10 @@
         <v>285</v>
       </c>
       <c r="E28" s="31" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="G28" s="25"/>
       <c r="H28" s="25"/>
@@ -6554,10 +6588,10 @@
         <v>285</v>
       </c>
       <c r="E29" s="31" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="G29" s="25"/>
       <c r="H29" s="25"/>
@@ -6573,16 +6607,16 @@
       <c r="A30" s="18"/>
       <c r="B30" s="29"/>
       <c r="C30" s="30" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D30" s="40" t="s">
-        <v>112</v>
+        <v>44</v>
       </c>
       <c r="E30" s="31" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>632</v>
+        <v>671</v>
       </c>
       <c r="G30" s="25"/>
       <c r="H30" s="25"/>
@@ -6596,20 +6630,18 @@
     </row>
     <row r="31" ht="23" customHeight="1" spans="1:15">
       <c r="A31" s="18"/>
-      <c r="B31" s="41" t="s">
-        <v>674</v>
-      </c>
+      <c r="B31" s="29"/>
       <c r="C31" s="30" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="D31" s="40" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>29</v>
+        <v>642</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>659</v>
+        <v>672</v>
       </c>
       <c r="G31" s="25"/>
       <c r="H31" s="25"/>
@@ -6623,18 +6655,18 @@
     </row>
     <row r="32" ht="23" customHeight="1" spans="1:15">
       <c r="A32" s="18"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="43" t="s">
-        <v>260</v>
-      </c>
-      <c r="E32" s="35" t="s">
-        <v>631</v>
+      <c r="B32" s="29"/>
+      <c r="C32" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="40" t="s">
+        <v>285</v>
+      </c>
+      <c r="E32" s="31" t="s">
+        <v>673</v>
       </c>
       <c r="F32" s="25" t="s">
-        <v>646</v>
+        <v>674</v>
       </c>
       <c r="G32" s="25"/>
       <c r="H32" s="25"/>
@@ -6648,11 +6680,19 @@
     </row>
     <row r="33" ht="23" customHeight="1" spans="1:15">
       <c r="A33" s="18"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="40" t="s">
+        <v>285</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>675</v>
+      </c>
+      <c r="F33" s="25" t="s">
+        <v>676</v>
+      </c>
       <c r="G33" s="25"/>
       <c r="H33" s="25"/>
       <c r="I33" s="25"/>
@@ -6665,11 +6705,19 @@
     </row>
     <row r="34" ht="23" customHeight="1" spans="1:15">
       <c r="A34" s="18"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" s="31" t="s">
+        <v>677</v>
+      </c>
+      <c r="F34" s="25" t="s">
+        <v>632</v>
+      </c>
       <c r="G34" s="25"/>
       <c r="H34" s="25"/>
       <c r="I34" s="25"/>
@@ -6682,11 +6730,21 @@
     </row>
     <row r="35" ht="23" customHeight="1" spans="1:15">
       <c r="A35" s="18"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
+      <c r="B35" s="41" t="s">
+        <v>678</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" s="25" t="s">
+        <v>663</v>
+      </c>
       <c r="G35" s="25"/>
       <c r="H35" s="25"/>
       <c r="I35" s="25"/>
@@ -6699,11 +6757,19 @@
     </row>
     <row r="36" ht="23" customHeight="1" spans="1:15">
       <c r="A36" s="18"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="43" t="s">
+        <v>260</v>
+      </c>
+      <c r="E36" s="35" t="s">
+        <v>631</v>
+      </c>
+      <c r="F36" s="25" t="s">
+        <v>646</v>
+      </c>
       <c r="G36" s="25"/>
       <c r="H36" s="25"/>
       <c r="I36" s="25"/>
@@ -9553,6 +9619,74 @@
       <c r="N203" s="22"/>
       <c r="O203" s="21"/>
     </row>
+    <row r="204" ht="23" customHeight="1" spans="1:15">
+      <c r="A204" s="18"/>
+      <c r="B204" s="19"/>
+      <c r="C204" s="24"/>
+      <c r="D204" s="25"/>
+      <c r="E204" s="25"/>
+      <c r="F204" s="25"/>
+      <c r="G204" s="25"/>
+      <c r="H204" s="25"/>
+      <c r="I204" s="25"/>
+      <c r="J204" s="32"/>
+      <c r="K204" s="21"/>
+      <c r="L204" s="22"/>
+      <c r="M204" s="20"/>
+      <c r="N204" s="22"/>
+      <c r="O204" s="21"/>
+    </row>
+    <row r="205" ht="23" customHeight="1" spans="1:15">
+      <c r="A205" s="18"/>
+      <c r="B205" s="19"/>
+      <c r="C205" s="24"/>
+      <c r="D205" s="25"/>
+      <c r="E205" s="25"/>
+      <c r="F205" s="25"/>
+      <c r="G205" s="25"/>
+      <c r="H205" s="25"/>
+      <c r="I205" s="25"/>
+      <c r="J205" s="32"/>
+      <c r="K205" s="21"/>
+      <c r="L205" s="22"/>
+      <c r="M205" s="20"/>
+      <c r="N205" s="22"/>
+      <c r="O205" s="21"/>
+    </row>
+    <row r="206" ht="23" customHeight="1" spans="1:15">
+      <c r="A206" s="18"/>
+      <c r="B206" s="19"/>
+      <c r="C206" s="24"/>
+      <c r="D206" s="25"/>
+      <c r="E206" s="25"/>
+      <c r="F206" s="25"/>
+      <c r="G206" s="25"/>
+      <c r="H206" s="25"/>
+      <c r="I206" s="25"/>
+      <c r="J206" s="32"/>
+      <c r="K206" s="21"/>
+      <c r="L206" s="22"/>
+      <c r="M206" s="20"/>
+      <c r="N206" s="22"/>
+      <c r="O206" s="21"/>
+    </row>
+    <row r="207" ht="23" customHeight="1" spans="1:15">
+      <c r="A207" s="18"/>
+      <c r="B207" s="19"/>
+      <c r="C207" s="24"/>
+      <c r="D207" s="25"/>
+      <c r="E207" s="25"/>
+      <c r="F207" s="25"/>
+      <c r="G207" s="25"/>
+      <c r="H207" s="25"/>
+      <c r="I207" s="25"/>
+      <c r="J207" s="32"/>
+      <c r="K207" s="21"/>
+      <c r="L207" s="22"/>
+      <c r="M207" s="20"/>
+      <c r="N207" s="22"/>
+      <c r="O207" s="21"/>
+    </row>
   </sheetData>
   <sheetProtection insertRows="0" insertHyperlinks="0" deleteRows="0"/>
   <mergeCells count="4">
@@ -9561,18 +9695,18 @@
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="L2:O2"/>
   </mergeCells>
-  <conditionalFormatting sqref="N104:N203">
+  <conditionalFormatting sqref="N108:N207">
     <cfRule type="beginsWith" dxfId="0" priority="1" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N104,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N108,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N104,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N108,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="3" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N104,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N108,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1 N3:N103">
+  <conditionalFormatting sqref="N1 N3:N107">
     <cfRule type="beginsWith" dxfId="0" priority="4" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N1,LEN("WARN"))="WARN"</formula>
     </cfRule>
@@ -9584,17 +9718,17 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15 C23 C30 C5:C14 C16:C22 C24:C29 C31:C203">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15 C18 C19 C20 C27 C34 C5:C14 C16:C17 C21:C22 C23:C26 C28:C33 C35:C207">
       <formula1>target</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D15 D23 D30 D5:D14 D16:D22 D24:D29 D31:D203">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D15 D18 D19 D20 D27 D34 D5:D14 D16:D17 D21:D22 D23:D26 D28:D33 D35:D207">
       <formula1>INDIRECT(C5)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="C22 C16" listDataValidation="1"/>
+    <ignoredError sqref="C26 C21" listDataValidation="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -9753,10 +9887,10 @@
         <v>386</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>675</v>
+        <v>679</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>676</v>
+        <v>680</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
@@ -9778,10 +9912,10 @@
         <v>386</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>677</v>
+        <v>681</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>678</v>
+        <v>682</v>
       </c>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
@@ -9803,10 +9937,10 @@
         <v>386</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>679</v>
+        <v>683</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>680</v>
+        <v>684</v>
       </c>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
@@ -9828,10 +9962,10 @@
         <v>386</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>681</v>
+        <v>685</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>682</v>
+        <v>686</v>
       </c>
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
@@ -9853,10 +9987,10 @@
         <v>386</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>683</v>
+        <v>687</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>684</v>
+        <v>688</v>
       </c>
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
@@ -9870,7 +10004,7 @@
     </row>
     <row r="10" ht="23" customHeight="1" spans="1:15">
       <c r="A10" s="18" t="s">
-        <v>685</v>
+        <v>689</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="24" t="s">
@@ -9880,7 +10014,7 @@
         <v>502</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>686</v>
+        <v>690</v>
       </c>
       <c r="F10" s="25"/>
       <c r="G10" s="25"/>
@@ -9903,10 +10037,10 @@
         <v>604</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>687</v>
+        <v>691</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>688</v>
+        <v>692</v>
       </c>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
@@ -9928,10 +10062,10 @@
         <v>604</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>689</v>
+        <v>693</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>688</v>
+        <v>692</v>
       </c>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
@@ -9953,13 +10087,13 @@
         <v>524</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>690</v>
+        <v>694</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>689</v>
+        <v>693</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>691</v>
+        <v>695</v>
       </c>
       <c r="H13" s="25"/>
       <c r="I13" s="25"/>
@@ -9972,7 +10106,7 @@
     </row>
     <row r="14" ht="23" customHeight="1" spans="1:15">
       <c r="A14" s="18" t="s">
-        <v>692</v>
+        <v>696</v>
       </c>
       <c r="B14" s="19"/>
       <c r="C14" s="24" t="s">
@@ -9982,10 +10116,10 @@
         <v>44</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>693</v>
+        <v>697</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>694</v>
+        <v>698</v>
       </c>
       <c r="G14" s="25"/>
       <c r="H14" s="25"/>
@@ -13120,7 +13254,7 @@
         <v>641</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>695</v>
+        <v>699</v>
       </c>
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
@@ -13210,10 +13344,10 @@
     </row>
     <row r="14" ht="23" customHeight="1" spans="1:15">
       <c r="A14" s="18" t="s">
-        <v>696</v>
+        <v>700</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>650</v>
+        <v>660</v>
       </c>
       <c r="C14" s="24" t="s">
         <v>29</v>
@@ -13222,16 +13356,16 @@
         <v>123</v>
       </c>
       <c r="E14" s="25" t="s">
+        <v>649</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>701</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>650</v>
+      </c>
+      <c r="H14" s="25" t="s">
         <v>651</v>
-      </c>
-      <c r="F14" s="36" t="s">
-        <v>697</v>
-      </c>
-      <c r="G14" s="25" t="s">
-        <v>652</v>
-      </c>
-      <c r="H14" s="25" t="s">
-        <v>653</v>
       </c>
       <c r="I14" s="25"/>
       <c r="J14" s="32"/>
@@ -13251,7 +13385,7 @@
         <v>426</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="F15" s="25"/>
       <c r="G15" s="25"/>
@@ -13267,7 +13401,7 @@
     <row r="16" ht="23" customHeight="1" spans="1:15">
       <c r="A16" s="18"/>
       <c r="B16" s="19" t="s">
-        <v>655</v>
+        <v>702</v>
       </c>
       <c r="C16" s="37" t="s">
         <v>17</v>
@@ -13276,7 +13410,7 @@
         <v>139</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="F16" s="25" t="s">
         <v>637</v>
@@ -13294,7 +13428,7 @@
     <row r="17" ht="23" customHeight="1" spans="1:15">
       <c r="A17" s="18"/>
       <c r="B17" s="19" t="s">
-        <v>698</v>
+        <v>703</v>
       </c>
       <c r="C17" s="24" t="s">
         <v>5</v>
@@ -13303,10 +13437,10 @@
         <v>386</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>699</v>
+        <v>704</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>700</v>
+        <v>705</v>
       </c>
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
@@ -13346,7 +13480,7 @@
     <row r="19" ht="23" customHeight="1" spans="1:15">
       <c r="A19" s="18"/>
       <c r="B19" s="26" t="s">
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="C19" s="27" t="s">
         <v>5</v>
@@ -13355,7 +13489,7 @@
         <v>382</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>701</v>
+        <v>706</v>
       </c>
       <c r="F19" s="25" t="s">
         <v>635</v>
@@ -13383,7 +13517,7 @@
         <v>636</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>702</v>
+        <v>707</v>
       </c>
       <c r="G20" s="25"/>
       <c r="H20" s="25"/>
@@ -13408,10 +13542,10 @@
         <v>16</v>
       </c>
       <c r="F21" s="36" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>659</v>
+        <v>663</v>
       </c>
       <c r="H21" s="25"/>
       <c r="I21" s="25"/>
@@ -13425,7 +13559,7 @@
     <row r="22" ht="23" customHeight="1" spans="1:15">
       <c r="A22" s="18"/>
       <c r="B22" s="29" t="s">
-        <v>661</v>
+        <v>665</v>
       </c>
       <c r="C22" s="30" t="s">
         <v>5</v>
@@ -13434,7 +13568,7 @@
         <v>265</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>662</v>
+        <v>666</v>
       </c>
       <c r="F22" s="25"/>
       <c r="G22" s="25"/>
@@ -13457,10 +13591,10 @@
         <v>285</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>664</v>
+        <v>668</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>665</v>
+        <v>669</v>
       </c>
       <c r="G23" s="25"/>
       <c r="H23" s="25"/>
@@ -13482,10 +13616,10 @@
         <v>44</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>666</v>
+        <v>670</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>667</v>
+        <v>671</v>
       </c>
       <c r="G24" s="25"/>
       <c r="H24" s="25"/>
@@ -13507,10 +13641,10 @@
         <v>44</v>
       </c>
       <c r="E25" s="31" t="s">
-        <v>695</v>
+        <v>699</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>668</v>
+        <v>672</v>
       </c>
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
@@ -13532,10 +13666,10 @@
         <v>285</v>
       </c>
       <c r="E26" s="31" t="s">
-        <v>669</v>
+        <v>673</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>670</v>
+        <v>674</v>
       </c>
       <c r="G26" s="25"/>
       <c r="H26" s="25"/>
@@ -13557,10 +13691,10 @@
         <v>285</v>
       </c>
       <c r="E27" s="31" t="s">
-        <v>671</v>
+        <v>675</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>672</v>
+        <v>676</v>
       </c>
       <c r="G27" s="25"/>
       <c r="H27" s="25"/>
@@ -13575,7 +13709,7 @@
     <row r="28" ht="23" customHeight="1" spans="1:15">
       <c r="A28" s="18"/>
       <c r="B28" s="41" t="s">
-        <v>674</v>
+        <v>678</v>
       </c>
       <c r="C28" s="30" t="s">
         <v>29</v>
@@ -13584,10 +13718,10 @@
         <v>62</v>
       </c>
       <c r="E28" s="42" t="s">
-        <v>697</v>
+        <v>701</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>659</v>
+        <v>663</v>
       </c>
       <c r="G28" s="25"/>
       <c r="H28" s="25"/>

</xml_diff>

<commit_message>
update failed test due to web page changes on mailinator
Signed-off-by: automike <mike.liu@covetrus.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_webmail.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_webmail.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28770" windowHeight="12435" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="19590" windowHeight="12495" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -2117,13 +2117,13 @@
     <t>loc.nav-items</t>
   </si>
   <si>
-    <t>css=.wrapper-nav-items a</t>
+    <t>css=nav #main-menu a</t>
   </si>
   <si>
     <t>loc.email-link</t>
   </si>
   <si>
-    <t>css=.wrapper-nav-items a[aria-label='Email']</t>
+    <t>css=header .container a.inbox-link</t>
   </si>
   <si>
     <t>expected.email-link</t>
@@ -2195,9 +2195,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -2268,8 +2268,22 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2288,34 +2302,6 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2343,24 +2329,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2382,16 +2359,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2405,14 +2375,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2439,13 +2439,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.05"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2457,67 +2457,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2541,7 +2487,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2553,19 +2511,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2577,55 +2595,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2759,21 +2753,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -2803,22 +2782,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2828,6 +2802,15 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2846,16 +2829,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2867,132 +2861,132 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="35" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3189,16 +3183,8 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -5817,10 +5803,10 @@
   <sheetPr/>
   <dimension ref="A1:O207"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="15"/>
@@ -6299,13 +6285,13 @@
       <c r="B18" s="54" t="s">
         <v>654</v>
       </c>
-      <c r="C18" s="55" t="s">
+      <c r="C18" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="56" t="s">
+      <c r="D18" s="40" t="s">
         <v>382</v>
       </c>
-      <c r="E18" s="56" t="s">
+      <c r="E18" s="40" t="s">
         <v>655</v>
       </c>
       <c r="F18" s="25" t="s">
@@ -6324,10 +6310,10 @@
     <row r="19" ht="23" customHeight="1" spans="1:15">
       <c r="A19" s="18"/>
       <c r="B19" s="54"/>
-      <c r="C19" s="55" t="s">
+      <c r="C19" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="56" t="s">
+      <c r="D19" s="40" t="s">
         <v>139</v>
       </c>
       <c r="E19" s="25" t="s">
@@ -6351,10 +6337,10 @@
       <c r="B20" s="54" t="s">
         <v>658</v>
       </c>
-      <c r="C20" s="55" t="s">
+      <c r="C20" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="56" t="s">
+      <c r="D20" s="40" t="s">
         <v>429</v>
       </c>
       <c r="E20" s="25" t="s">
@@ -6375,10 +6361,10 @@
       <c r="B21" s="54" t="s">
         <v>660</v>
       </c>
-      <c r="C21" s="55" t="s">
+      <c r="C21" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="56" t="s">
+      <c r="D21" s="40" t="s">
         <v>123</v>
       </c>
       <c r="E21" s="25" t="s">
@@ -6404,10 +6390,10 @@
     <row r="22" ht="23" customHeight="1" spans="1:15">
       <c r="A22" s="18"/>
       <c r="B22" s="54"/>
-      <c r="C22" s="55" t="s">
+      <c r="C22" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="56" t="s">
+      <c r="D22" s="40" t="s">
         <v>426</v>
       </c>
       <c r="E22" s="25" t="s">
@@ -9728,7 +9714,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="C26 C21" listDataValidation="1"/>
+    <ignoredError sqref="C21 C26" listDataValidation="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -9738,10 +9724,10 @@
   <sheetPr/>
   <dimension ref="A1:O178"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="15"/>

</xml_diff>